<commit_message>
fix: Eliminar selector de banco - detectar banco desde columna Excel
</commit_message>
<xml_diff>
--- a/test_upload.xlsx
+++ b/test_upload.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -447,6 +447,11 @@
           <t>Detalle</t>
         </is>
       </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Banco</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -472,6 +477,11 @@
           <t>Mercado D1</t>
         </is>
       </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Bancolombia</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -497,6 +507,11 @@
           <t>Gasolina</t>
         </is>
       </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Itau</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -522,6 +537,11 @@
           <t>Nómina Febrero</t>
         </is>
       </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Bancolombia</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -547,6 +567,11 @@
           <t>Netflix</t>
         </is>
       </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Itau</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -570,6 +595,11 @@
       <c r="E6" t="inlineStr">
         <is>
           <t>Farmacia</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Davivienda</t>
         </is>
       </c>
     </row>

</xml_diff>